<commit_message>
change in pack as no supplier stock report is not in SNCH module
</commit_message>
<xml_diff>
--- a/Library/excelTestCasesTestPackPharmacyReports_SNCH.xlsx
+++ b/Library/excelTestCasesTestPackPharmacyReports_SNCH.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -54,9 +54,6 @@
     <t>TC009</t>
   </si>
   <si>
-    <t>TC010</t>
-  </si>
-  <si>
     <t>TC011</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
   </si>
   <si>
     <t>Pharmacy\Reports\Sales\TC07SalesSummaryReport.py</t>
-  </si>
-  <si>
-    <t>Pharmacy\Reports\Stock\TC01SupplierStockReport.py</t>
   </si>
   <si>
     <t>Pharmacy\Reports\Stock\TC02ExpiryReport.py</t>
@@ -483,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +504,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -519,21 +513,21 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -544,40 +538,40 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" s="3">
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -588,18 +582,18 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -610,21 +604,21 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -635,18 +629,18 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
@@ -657,18 +651,18 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -679,18 +673,18 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -701,51 +695,29 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change in excelTestCasesTestPackPharmacyReports_SNCH.xlsx added return to supplier report
</commit_message>
<xml_diff>
--- a/Library/excelTestCasesTestPackPharmacyReports_SNCH.xlsx
+++ b/Library/excelTestCasesTestPackPharmacyReports_SNCH.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>TC012</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Purchase\TC03ReturnToSupplierReport.py</t>
+  </si>
+  <si>
+    <t>TC03</t>
   </si>
 </sst>
 </file>
@@ -477,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +571,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
@@ -577,7 +583,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -587,7 +593,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
@@ -599,20 +605,17 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J5" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>12</v>
@@ -624,17 +627,20 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>12</v>
@@ -646,7 +652,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -656,7 +662,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>12</v>
@@ -668,7 +674,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -678,7 +684,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>12</v>
@@ -690,7 +696,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -700,7 +706,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>12</v>
@@ -712,11 +718,33 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="1" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added stock transfer report in excelTestCasesTestPackPharmacyReports_SNCH.xlsx and manage LibModulePharmacy.py accordingly
</commit_message>
<xml_diff>
--- a/Library/excelTestCasesTestPackPharmacyReports_SNCH.xlsx
+++ b/Library/excelTestCasesTestPackPharmacyReports_SNCH.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>TC03</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Stock\StockTransferReport.py</t>
+  </si>
+  <si>
+    <t>TC013</t>
   </si>
 </sst>
 </file>
@@ -190,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -198,6 +204,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,6 +755,28 @@
         <v>27</v>
       </c>
     </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added Narcotics Stock report in pack
</commit_message>
<xml_diff>
--- a/Library/excelTestCasesTestPackPharmacyReports_SNCH.xlsx
+++ b/Library/excelTestCasesTestPackPharmacyReports_SNCH.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="36">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>TC013</t>
+  </si>
+  <si>
+    <t>TC014</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Stock\TC04NarcoticStockReport.py</t>
   </si>
 </sst>
 </file>
@@ -490,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,6 +783,28 @@
         <v>27</v>
       </c>
     </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>